<commit_message>
Implemented 2.1 and 2.2
</commit_message>
<xml_diff>
--- a/docu/groupUpdateTemplate.xlsx
+++ b/docu/groupUpdateTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruwantennakoon/Teaching/2022/COSC1076/Assignments/A2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\dev\school\y2\adv_prog\ass\ap_ass2\docu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D69252C8-F6F8-8448-85EA-3FAE931ED2FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA88B5B7-718B-4582-8A33-603E9F8D49B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33900" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="49">
   <si>
     <t>Assignment 2 | Weekly Update Tracking Sheet</t>
   </si>
@@ -163,13 +163,28 @@
   </si>
   <si>
     <t>Gameplay for single round</t>
+  </si>
+  <si>
+    <t>Rafat Mahiuddin</t>
+  </si>
+  <si>
+    <t>Created a group of 3, a MS Teams group chat and a github repo.</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Completed main menu implementation.</t>
+  </si>
+  <si>
+    <t>Implemented standard error checking for player names and files.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -189,8 +204,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -201,6 +223,11 @@
       <patternFill patternType="solid">
         <fgColor indexed="16"/>
         <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -503,10 +530,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -571,8 +599,11 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
@@ -1838,24 +1869,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.95" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="14.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.125" style="1" customWidth="1"/>
     <col min="4" max="4" width="62.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="30.83203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="30.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.625" style="1" customWidth="1"/>
     <col min="7" max="10" width="41.5" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.83203125" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.83203125" style="1"/>
+    <col min="11" max="11" width="10.875" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="24" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>42</v>
       </c>
@@ -1869,7 +1900,7 @@
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
     </row>
-    <row r="2" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="24" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1883,7 +1914,7 @@
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
     </row>
-    <row r="3" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="15.2" customHeight="1">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1895,7 +1926,7 @@
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="15.2" customHeight="1">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -1909,12 +1940,12 @@
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="15.2" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="4" t="s">
@@ -1929,7 +1960,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="15.2" customHeight="1">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
@@ -1947,7 +1978,7 @@
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="15.2" customHeight="1">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -1965,7 +1996,7 @@
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
     </row>
-    <row r="8" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="15.2" customHeight="1">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
@@ -1983,7 +2014,7 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
     </row>
-    <row r="9" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="15.2" customHeight="1">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
@@ -1997,7 +2028,7 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="15.2" customHeight="1">
       <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
@@ -2011,7 +2042,7 @@
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
     </row>
-    <row r="11" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="15.2" customHeight="1">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="6"/>
@@ -2023,7 +2054,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
     </row>
-    <row r="12" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="15.2" customHeight="1">
       <c r="A12" s="3"/>
       <c r="B12" s="7"/>
       <c r="C12" s="8" t="s">
@@ -2040,7 +2071,7 @@
       </c>
       <c r="G12" s="8" t="str">
         <f>$B$5</f>
-        <v>A</v>
+        <v>Rafat Mahiuddin</v>
       </c>
       <c r="H12" s="9" t="str">
         <f>$B$6</f>
@@ -2054,7 +2085,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A13" s="3"/>
       <c r="B13" s="7"/>
       <c r="C13" s="12"/>
@@ -2065,12 +2096,14 @@
       <c r="F13" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="16"/>
+      <c r="G13" s="16" t="s">
+        <v>45</v>
+      </c>
       <c r="H13" s="17"/>
       <c r="I13" s="14"/>
       <c r="J13" s="14"/>
     </row>
-    <row r="14" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A14" s="3"/>
       <c r="B14" s="7"/>
       <c r="C14" s="18"/>
@@ -2081,12 +2114,14 @@
       <c r="F14" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="22"/>
+      <c r="G14" s="22" t="s">
+        <v>46</v>
+      </c>
       <c r="H14" s="23"/>
       <c r="I14" s="20"/>
       <c r="J14" s="20"/>
     </row>
-    <row r="15" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A15" s="3"/>
       <c r="B15" s="7"/>
       <c r="C15" s="18"/>
@@ -2102,7 +2137,7 @@
       <c r="I15" s="20"/>
       <c r="J15" s="20"/>
     </row>
-    <row r="16" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A16" s="3"/>
       <c r="B16" s="7"/>
       <c r="C16" s="18"/>
@@ -2114,7 +2149,7 @@
       <c r="I16" s="20"/>
       <c r="J16" s="20"/>
     </row>
-    <row r="17" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A17" s="3"/>
       <c r="B17" s="7"/>
       <c r="C17" s="18"/>
@@ -2125,7 +2160,7 @@
       <c r="I17" s="20"/>
       <c r="J17" s="20"/>
     </row>
-    <row r="18" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="15.2" customHeight="1">
       <c r="A18" s="3"/>
       <c r="B18" s="7"/>
       <c r="C18" s="25"/>
@@ -2137,23 +2172,23 @@
       <c r="I18" s="20"/>
       <c r="J18" s="20"/>
     </row>
-    <row r="19" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="15.2" customHeight="1">
       <c r="A19" s="3"/>
       <c r="B19" s="7"/>
       <c r="C19" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="39"/>
+      <c r="D19" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="41"/>
       <c r="F19" s="28"/>
       <c r="G19" s="29"/>
       <c r="H19" s="26"/>
       <c r="I19" s="27"/>
       <c r="J19" s="27"/>
     </row>
-    <row r="20" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="15.2" customHeight="1">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="30"/>
@@ -2165,7 +2200,7 @@
       <c r="I20" s="30"/>
       <c r="J20" s="30"/>
     </row>
-    <row r="21" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="15.2" customHeight="1">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="6"/>
@@ -2177,7 +2212,7 @@
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
     </row>
-    <row r="22" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="15.2" customHeight="1">
       <c r="A22" s="3"/>
       <c r="B22" s="7"/>
       <c r="C22" s="8" t="s">
@@ -2194,7 +2229,7 @@
       </c>
       <c r="G22" s="8" t="str">
         <f>$B$5</f>
-        <v>A</v>
+        <v>Rafat Mahiuddin</v>
       </c>
       <c r="H22" s="9" t="str">
         <f>$B$6</f>
@@ -2208,7 +2243,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="15.2" customHeight="1">
       <c r="A23" s="3"/>
       <c r="B23" s="7"/>
       <c r="C23" s="35"/>
@@ -2224,7 +2259,7 @@
       <c r="I23" s="37"/>
       <c r="J23" s="37"/>
     </row>
-    <row r="24" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A24" s="3"/>
       <c r="B24" s="7"/>
       <c r="C24" s="12"/>
@@ -2240,7 +2275,7 @@
       <c r="I24" s="14"/>
       <c r="J24" s="14"/>
     </row>
-    <row r="25" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A25" s="3"/>
       <c r="B25" s="7"/>
       <c r="C25" s="18"/>
@@ -2251,12 +2286,14 @@
       <c r="F25" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="G25" s="22"/>
+      <c r="G25" s="22" t="s">
+        <v>47</v>
+      </c>
       <c r="H25" s="23"/>
       <c r="I25" s="20"/>
       <c r="J25" s="20"/>
     </row>
-    <row r="26" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A26" s="3"/>
       <c r="B26" s="7"/>
       <c r="C26" s="18"/>
@@ -2264,12 +2301,14 @@
         <v>28</v>
       </c>
       <c r="E26" s="7"/>
-      <c r="G26" s="22"/>
+      <c r="G26" s="22" t="s">
+        <v>48</v>
+      </c>
       <c r="H26" s="23"/>
       <c r="I26" s="20"/>
       <c r="J26" s="20"/>
     </row>
-    <row r="27" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A27" s="3"/>
       <c r="B27" s="7"/>
       <c r="C27" s="18"/>
@@ -2283,7 +2322,7 @@
       <c r="I27" s="20"/>
       <c r="J27" s="20"/>
     </row>
-    <row r="28" spans="1:10" ht="30.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="30.2" customHeight="1">
       <c r="A28" s="3"/>
       <c r="B28" s="7"/>
       <c r="C28" s="18"/>
@@ -2297,7 +2336,7 @@
       <c r="I28" s="20"/>
       <c r="J28" s="20"/>
     </row>
-    <row r="29" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="15.2" customHeight="1">
       <c r="A29" s="3"/>
       <c r="B29" s="7"/>
       <c r="C29" s="18"/>
@@ -2311,7 +2350,7 @@
       <c r="I29" s="20"/>
       <c r="J29" s="20"/>
     </row>
-    <row r="30" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" ht="15.2" customHeight="1">
       <c r="A30" s="3"/>
       <c r="B30" s="7"/>
       <c r="C30" s="25"/>
@@ -2323,7 +2362,7 @@
       <c r="I30" s="20"/>
       <c r="J30" s="20"/>
     </row>
-    <row r="31" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="15.2" customHeight="1">
       <c r="A31" s="3"/>
       <c r="B31" s="7"/>
       <c r="C31" s="8" t="s">
@@ -2339,7 +2378,7 @@
       <c r="I31" s="27"/>
       <c r="J31" s="27"/>
     </row>
-    <row r="32" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="15.2" customHeight="1">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="30"/>
@@ -2351,7 +2390,7 @@
       <c r="I32" s="30"/>
       <c r="J32" s="30"/>
     </row>
-    <row r="33" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" ht="15.2" customHeight="1">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="6"/>
@@ -2363,7 +2402,7 @@
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>
     </row>
-    <row r="34" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" ht="15.2" customHeight="1">
       <c r="A34" s="3"/>
       <c r="B34" s="7"/>
       <c r="C34" s="8" t="s">
@@ -2391,7 +2430,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" ht="33.950000000000003" customHeight="1">
       <c r="A35" s="3"/>
       <c r="B35" s="7"/>
       <c r="C35" s="12"/>
@@ -2407,7 +2446,7 @@
       <c r="I35" s="14"/>
       <c r="J35" s="14"/>
     </row>
-    <row r="36" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A36" s="3"/>
       <c r="B36" s="7"/>
       <c r="C36" s="18"/>
@@ -2423,7 +2462,7 @@
       <c r="I36" s="20"/>
       <c r="J36" s="20"/>
     </row>
-    <row r="37" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" ht="15.2" customHeight="1">
       <c r="A37" s="3"/>
       <c r="B37" s="7"/>
       <c r="C37" s="18"/>
@@ -2439,7 +2478,7 @@
       <c r="I37" s="20"/>
       <c r="J37" s="20"/>
     </row>
-    <row r="38" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" ht="15.75">
       <c r="A38" s="3"/>
       <c r="B38" s="7"/>
       <c r="C38" s="18"/>
@@ -2453,7 +2492,7 @@
       <c r="I38" s="20"/>
       <c r="J38" s="20"/>
     </row>
-    <row r="39" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A39" s="3"/>
       <c r="B39" s="7"/>
       <c r="C39" s="18"/>
@@ -2465,7 +2504,7 @@
       <c r="I39" s="20"/>
       <c r="J39" s="20"/>
     </row>
-    <row r="40" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" ht="15.2" customHeight="1">
       <c r="A40" s="3"/>
       <c r="B40" s="7"/>
       <c r="C40" s="25"/>
@@ -2477,7 +2516,7 @@
       <c r="I40" s="20"/>
       <c r="J40" s="20"/>
     </row>
-    <row r="41" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" ht="15.2" customHeight="1">
       <c r="A41" s="3"/>
       <c r="B41" s="7"/>
       <c r="C41" s="8" t="s">
@@ -2493,7 +2532,7 @@
       <c r="I41" s="27"/>
       <c r="J41" s="27"/>
     </row>
-    <row r="42" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" ht="15.2" customHeight="1">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="30"/>
@@ -2505,7 +2544,7 @@
       <c r="I42" s="30"/>
       <c r="J42" s="30"/>
     </row>
-    <row r="43" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" ht="15.2" customHeight="1">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="6"/>
@@ -2517,7 +2556,7 @@
       <c r="I43" s="6"/>
       <c r="J43" s="6"/>
     </row>
-    <row r="44" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" ht="15.2" customHeight="1">
       <c r="A44" s="3"/>
       <c r="B44" s="7"/>
       <c r="C44" s="8" t="s">
@@ -2545,7 +2584,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A45" s="3"/>
       <c r="B45" s="7"/>
       <c r="C45" s="12"/>
@@ -2561,7 +2600,7 @@
       <c r="I45" s="14"/>
       <c r="J45" s="14"/>
     </row>
-    <row r="46" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" ht="15.2" customHeight="1">
       <c r="A46" s="3"/>
       <c r="B46" s="7"/>
       <c r="C46" s="18"/>
@@ -2577,7 +2616,7 @@
       <c r="I46" s="20"/>
       <c r="J46" s="20"/>
     </row>
-    <row r="47" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A47" s="3"/>
       <c r="B47" s="7"/>
       <c r="C47" s="18"/>
@@ -2591,7 +2630,7 @@
       <c r="I47" s="20"/>
       <c r="J47" s="20"/>
     </row>
-    <row r="48" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A48" s="3"/>
       <c r="B48" s="7"/>
       <c r="C48" s="18"/>
@@ -2605,7 +2644,7 @@
       <c r="I48" s="20"/>
       <c r="J48" s="20"/>
     </row>
-    <row r="49" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A49" s="3"/>
       <c r="B49" s="7"/>
       <c r="C49" s="18"/>
@@ -2619,7 +2658,7 @@
       <c r="I49" s="20"/>
       <c r="J49" s="20"/>
     </row>
-    <row r="50" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" ht="15.2" customHeight="1">
       <c r="A50" s="3"/>
       <c r="B50" s="7"/>
       <c r="C50" s="25"/>
@@ -2631,7 +2670,7 @@
       <c r="I50" s="20"/>
       <c r="J50" s="20"/>
     </row>
-    <row r="51" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" ht="15.2" customHeight="1">
       <c r="A51" s="3"/>
       <c r="B51" s="7"/>
       <c r="C51" s="8" t="s">
@@ -2647,7 +2686,7 @@
       <c r="I51" s="27"/>
       <c r="J51" s="27"/>
     </row>
-    <row r="52" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" ht="15.2" customHeight="1">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="30"/>
@@ -2659,7 +2698,7 @@
       <c r="I52" s="30"/>
       <c r="J52" s="30"/>
     </row>
-    <row r="53" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" ht="15.2" customHeight="1">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="6"/>

</xml_diff>